<commit_message>
Add new fastq_qc-analysis data delivery option
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1603.11.microbial.xlsx
+++ b/tests/fixtures/orderforms/1603.11.microbial.xlsx
@@ -8,24 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik.grenfeldt/Documents/GitHub/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B8AFC8-24D1-F449-A273-705C0CA23EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E733D8-0066-7441-99D0-29FB0EB32AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="27840" windowHeight="17500" tabRatio="593" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="-21100" windowWidth="28800" windowHeight="21100" tabRatio="593" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="6" r:id="rId1"/>
     <sheet name="order form" sheetId="1" r:id="rId2"/>
     <sheet name="Drop down list" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="463">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1619,12 +1612,6 @@
     </r>
   </si>
   <si>
-    <t>Fastq QC + Analysis + Cram</t>
-  </si>
-  <si>
-    <t>Updated options for "Delivery" to: Fastq QC and Fastq QC + Analysis + Cram</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Data Delivery: </t>
     </r>
@@ -1679,12 +1666,12 @@
     </r>
   </si>
   <si>
+    <t>UDF/Controls</t>
+  </si>
+  <si>
     <t>Controls</t>
   </si>
   <si>
-    <t>blank</t>
-  </si>
-  <si>
     <t>positive</t>
   </si>
   <si>
@@ -1694,12 +1681,6 @@
     <t>priority</t>
   </si>
   <si>
-    <t>Added "Controls" with options blank, positive, negative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added stauts priority for "Priority" </t>
-  </si>
-  <si>
     <t>Removed Application tags: MWGNXTR003, MWMNXTR003, MWLNXTR003 and VWGDPTR001</t>
   </si>
   <si>
@@ -1707,7 +1688,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Controls: </t>
+      <t>Volume (uL):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The volume of the sample in uL. Do not include the unit in the form!</t>
+    </r>
+  </si>
+  <si>
+    <t>Control sample</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Control sample: </t>
     </r>
     <r>
       <rPr>
@@ -1716,7 +1713,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Indicating if samples are control samples or not. Options available in drop down list: blank (no control), positive, negative.</t>
+      <t>Indicating if a sample is a control (positive/negative) or not. Options available in drop down list: blank (" ", not a control), positive, negative.</t>
     </r>
     <r>
       <rPr>
@@ -1731,113 +1728,109 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Volume (uL):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> The volume of the sample in uL. Do not include the unit in the form!</t>
-    </r>
+    <t xml:space="preserve">Added status priority for "Priority" </t>
+  </si>
+  <si>
+    <t>Added "Control sample" with options blank (" "), positive, negative</t>
+  </si>
+  <si>
+    <t>Fastq QC + Analysis</t>
+  </si>
+  <si>
+    <t>Updated options for "Delivery" to: Fastq QC and Fastq QC + Analysis</t>
+  </si>
+  <si>
+    <t>NC_000001</t>
   </si>
   <si>
     <t>microbialsample1</t>
   </si>
   <si>
+    <t>microbialsample2</t>
+  </si>
+  <si>
+    <t>microbialsample3</t>
+  </si>
+  <si>
+    <t>microbialsample4</t>
+  </si>
+  <si>
+    <t>microbialsample5</t>
+  </si>
+  <si>
+    <t>microbialsample6</t>
+  </si>
+  <si>
+    <t>microbialsample7</t>
+  </si>
+  <si>
+    <t>microbialsample8</t>
+  </si>
+  <si>
+    <t>microbialsample9</t>
+  </si>
+  <si>
+    <t>microbialsample10</t>
+  </si>
+  <si>
+    <t>microbialsample11</t>
+  </si>
+  <si>
+    <t>microbialsample12</t>
+  </si>
+  <si>
+    <t>microbialsample13</t>
+  </si>
+  <si>
+    <t>microbialsample14</t>
+  </si>
+  <si>
+    <t>NC_000002</t>
+  </si>
+  <si>
+    <t>NC_000003</t>
+  </si>
+  <si>
+    <t>NC_000004</t>
+  </si>
+  <si>
+    <t>NC_000005</t>
+  </si>
+  <si>
+    <t>NC_000006</t>
+  </si>
+  <si>
+    <t>NC_000007</t>
+  </si>
+  <si>
+    <t>NC_000008</t>
+  </si>
+  <si>
+    <t>NC_000009</t>
+  </si>
+  <si>
+    <t>NC_000010</t>
+  </si>
+  <si>
+    <t>NC_000011</t>
+  </si>
+  <si>
+    <t>NC_000012</t>
+  </si>
+  <si>
+    <t>NC_000013</t>
+  </si>
+  <si>
+    <t>NC_000014</t>
+  </si>
+  <si>
     <t>other species</t>
   </si>
   <si>
-    <t>NC_000001</t>
-  </si>
-  <si>
-    <t>NC_000002</t>
-  </si>
-  <si>
-    <t>NC_000003</t>
-  </si>
-  <si>
-    <t>NC_000004</t>
-  </si>
-  <si>
-    <t>NC_000005</t>
-  </si>
-  <si>
-    <t>NC_000006</t>
-  </si>
-  <si>
-    <t>NC_000007</t>
-  </si>
-  <si>
-    <t>NC_000008</t>
-  </si>
-  <si>
-    <t>NC_000009</t>
-  </si>
-  <si>
-    <t>NC_000010</t>
-  </si>
-  <si>
-    <t>NC_000011</t>
-  </si>
-  <si>
-    <t>NC_000012</t>
-  </si>
-  <si>
-    <t>NC_000013</t>
-  </si>
-  <si>
-    <t>NC_000014</t>
+    <t>comments</t>
   </si>
   <si>
     <t>plate1</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>microbialsample2</t>
-  </si>
-  <si>
-    <t>microbialsample3</t>
-  </si>
-  <si>
-    <t>microbialsample4</t>
-  </si>
-  <si>
-    <t>microbialsample5</t>
-  </si>
-  <si>
-    <t>microbialsample6</t>
-  </si>
-  <si>
-    <t>microbialsample7</t>
-  </si>
-  <si>
-    <t>microbialsample8</t>
-  </si>
-  <si>
-    <t>microbialsample9</t>
-  </si>
-  <si>
-    <t>microbialsample10</t>
-  </si>
-  <si>
-    <t>microbialsample11</t>
-  </si>
-  <si>
-    <t>microbialsample12</t>
-  </si>
-  <si>
-    <t>microbialsample13</t>
-  </si>
-  <si>
-    <t>microbialsample14</t>
-  </si>
-  <si>
-    <t>UDF/Control</t>
   </si>
 </sst>
 </file>
@@ -3788,7 +3781,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3832,7 +3825,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3857,7 +3850,7 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3873,7 +3866,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D1" s="56"/>
       <c r="E1" s="21"/>
@@ -3930,17 +3923,17 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="57" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="57" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="80" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="14" x14ac:dyDescent="0.15">
@@ -3955,7 +3948,7 @@
     </row>
     <row r="21" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="80" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
@@ -4001,12 +3994,12 @@
     </row>
     <row r="31" spans="1:1" ht="49" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="122" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="71" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="67" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="47" customHeight="1" x14ac:dyDescent="0.15">
@@ -4023,7 +4016,7 @@
     </row>
     <row r="35" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="66" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C35" s="64"/>
       <c r="E35" s="64"/>
@@ -4052,7 +4045,7 @@
     <row r="40" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40"/>
     </row>
-    <row r="41" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="65" t="s">
         <v>250</v>
       </c>
@@ -4176,7 +4169,7 @@
       <c r="A75" s="64"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fuoacgz3pYOMyrTSr3D5fEbxCJ0+9jtNavhzecbzzkkpoKr6FmPGJ5KnGxv6Ft/0rjlABS9HHlDP094SGs6O3g==" saltValue="/Vj3erruPImpsS+F4zs2Lg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
@@ -4198,8 +4191,8 @@
   </sheetPr>
   <dimension ref="A1:W232"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4473,7 +4466,7 @@
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" s="1" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="s">
         <v>0</v>
       </c>
@@ -4500,7 +4493,7 @@
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
     </row>
-    <row r="11" spans="1:23" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" s="2" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -4511,7 +4504,7 @@
         <v>74</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>462</v>
+        <v>418</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>411</v>
@@ -4563,7 +4556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" s="3" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="22" t="s">
         <v>5</v>
       </c>
@@ -4601,7 +4594,7 @@
         <v>82</v>
       </c>
       <c r="D13" s="121" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="E13" s="118" t="s">
         <v>410</v>
@@ -4653,7 +4646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="3" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" s="3" customFormat="1" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
         <v>6</v>
       </c>
@@ -4682,19 +4675,19 @@
     </row>
     <row r="15" spans="1:23" s="48" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="83" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B15" s="129" t="s">
         <v>284</v>
       </c>
       <c r="C15" s="113" t="s">
-        <v>433</v>
-      </c>
-      <c r="D15" s="129" t="s">
-        <v>422</v>
+        <v>432</v>
+      </c>
+      <c r="D15" s="114" t="s">
+        <v>420</v>
       </c>
       <c r="E15" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F15" s="129" t="s">
         <v>262</v>
@@ -4702,7 +4695,7 @@
       <c r="G15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="113" t="s">
+      <c r="H15" s="129" t="s">
         <v>345</v>
       </c>
       <c r="I15" s="113" t="s">
@@ -4719,14 +4712,14 @@
       </c>
       <c r="M15" s="43"/>
       <c r="N15" s="44" t="s">
-        <v>447</v>
+        <v>462</v>
       </c>
       <c r="O15" s="120" t="s">
         <v>25</v>
       </c>
       <c r="P15" s="74"/>
       <c r="Q15" s="76" t="s">
-        <v>432</v>
+        <v>460</v>
       </c>
       <c r="R15" s="72"/>
       <c r="S15" s="82">
@@ -4736,7 +4729,7 @@
         <v>3</v>
       </c>
       <c r="U15" s="76" t="s">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="V15" s="46"/>
       <c r="W15" s="18" t="s">
@@ -4745,19 +4738,19 @@
     </row>
     <row r="16" spans="1:23" s="48" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="83" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="B16" s="129" t="s">
         <v>280</v>
       </c>
       <c r="C16" s="113" t="s">
-        <v>434</v>
-      </c>
-      <c r="D16" s="129" t="s">
-        <v>423</v>
+        <v>447</v>
+      </c>
+      <c r="D16" s="114" t="s">
+        <v>421</v>
       </c>
       <c r="E16" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F16" s="129" t="s">
         <v>289</v>
@@ -4765,7 +4758,7 @@
       <c r="G16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="113" t="s">
+      <c r="H16" s="129" t="s">
         <v>287</v>
       </c>
       <c r="I16" s="129" t="s">
@@ -4796,16 +4789,17 @@
     </row>
     <row r="17" spans="1:23" s="48" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="83" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="B17" s="129" t="s">
         <v>268</v>
       </c>
       <c r="C17" s="113" t="s">
-        <v>435</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="D17" s="114"/>
       <c r="E17" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F17" s="129" t="s">
         <v>290</v>
@@ -4813,7 +4807,7 @@
       <c r="G17" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="113" t="s">
+      <c r="H17" s="129" t="s">
         <v>344</v>
       </c>
       <c r="I17" s="129" t="s">
@@ -4823,7 +4817,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="129" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="L17" s="113" t="s">
         <v>90</v>
@@ -4844,17 +4838,17 @@
     </row>
     <row r="18" spans="1:23" s="48" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="83" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="B18" s="129" t="s">
         <v>269</v>
       </c>
       <c r="C18" s="113" t="s">
-        <v>436</v>
-      </c>
-      <c r="D18" s="129"/>
+        <v>449</v>
+      </c>
+      <c r="D18" s="114"/>
       <c r="E18" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F18" s="129" t="s">
         <v>291</v>
@@ -4862,8 +4856,8 @@
       <c r="G18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="113" t="s">
-        <v>344</v>
+      <c r="H18" s="129" t="s">
+        <v>287</v>
       </c>
       <c r="I18" s="129" t="s">
         <v>244</v>
@@ -4893,25 +4887,25 @@
     </row>
     <row r="19" spans="1:23" s="48" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="83" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="B19" s="129" t="s">
         <v>281</v>
       </c>
       <c r="C19" s="113" t="s">
-        <v>437</v>
-      </c>
-      <c r="D19" s="129"/>
+        <v>450</v>
+      </c>
+      <c r="D19" s="114"/>
       <c r="E19" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F19" s="129" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="113" t="s">
+      <c r="H19" s="129" t="s">
         <v>344</v>
       </c>
       <c r="I19" s="129" t="s">
@@ -4921,7 +4915,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="129" t="s">
-        <v>261</v>
+        <v>182</v>
       </c>
       <c r="L19" s="113" t="s">
         <v>90</v>
@@ -4942,26 +4936,26 @@
     </row>
     <row r="20" spans="1:23" s="48" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="83" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="B20" s="129" t="s">
         <v>282</v>
       </c>
       <c r="C20" s="113" t="s">
-        <v>438</v>
-      </c>
-      <c r="D20" s="129"/>
+        <v>451</v>
+      </c>
+      <c r="D20" s="114"/>
       <c r="E20" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F20" s="129" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="113" t="s">
-        <v>344</v>
+      <c r="H20" s="129" t="s">
+        <v>287</v>
       </c>
       <c r="I20" s="129" t="s">
         <v>402</v>
@@ -4970,7 +4964,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="129" t="s">
-        <v>261</v>
+        <v>18</v>
       </c>
       <c r="L20" s="113" t="s">
         <v>90</v>
@@ -4991,35 +4985,35 @@
     </row>
     <row r="21" spans="1:23" s="48" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="83" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="B21" s="129" t="s">
         <v>270</v>
       </c>
       <c r="C21" s="113" t="s">
-        <v>439</v>
-      </c>
-      <c r="D21" s="113"/>
+        <v>452</v>
+      </c>
+      <c r="D21" s="114"/>
       <c r="E21" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F21" s="129" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="113" t="s">
+      <c r="H21" s="129" t="s">
         <v>344</v>
       </c>
       <c r="I21" s="129" t="s">
-        <v>402</v>
+        <v>263</v>
       </c>
       <c r="J21" s="113">
         <v>1</v>
       </c>
       <c r="K21" s="129" t="s">
-        <v>261</v>
+        <v>422</v>
       </c>
       <c r="L21" s="113" t="s">
         <v>90</v>
@@ -5040,17 +5034,17 @@
     </row>
     <row r="22" spans="1:23" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="83" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="B22" s="129" t="s">
         <v>271</v>
       </c>
       <c r="C22" s="113" t="s">
-        <v>440</v>
-      </c>
-      <c r="D22" s="113"/>
+        <v>453</v>
+      </c>
+      <c r="D22" s="114"/>
       <c r="E22" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F22" s="129" t="s">
         <v>291</v>
@@ -5058,11 +5052,11 @@
       <c r="G22" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="113" t="s">
-        <v>344</v>
+      <c r="H22" s="129" t="s">
+        <v>287</v>
       </c>
       <c r="I22" s="129" t="s">
-        <v>402</v>
+        <v>243</v>
       </c>
       <c r="J22" s="113">
         <v>1</v>
@@ -5087,37 +5081,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="24" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="83" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="B23" s="129" t="s">
         <v>272</v>
       </c>
       <c r="C23" s="113" t="s">
-        <v>441</v>
-      </c>
-      <c r="D23" s="113"/>
+        <v>454</v>
+      </c>
+      <c r="D23" s="114"/>
       <c r="E23" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F23" s="129" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="113" t="s">
+      <c r="H23" s="129" t="s">
         <v>344</v>
       </c>
       <c r="I23" s="129" t="s">
-        <v>402</v>
+        <v>244</v>
       </c>
       <c r="J23" s="113">
         <v>1</v>
       </c>
       <c r="K23" s="129" t="s">
-        <v>261</v>
+        <v>182</v>
       </c>
       <c r="L23" s="113" t="s">
         <v>90</v>
@@ -5136,37 +5130,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="24" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="83" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="B24" s="129" t="s">
         <v>273</v>
       </c>
       <c r="C24" s="113" t="s">
-        <v>442</v>
-      </c>
-      <c r="D24" s="113"/>
+        <v>455</v>
+      </c>
+      <c r="D24" s="114"/>
       <c r="E24" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F24" s="129" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="113" t="s">
-        <v>344</v>
+      <c r="H24" s="129" t="s">
+        <v>287</v>
       </c>
       <c r="I24" s="129" t="s">
-        <v>402</v>
+        <v>245</v>
       </c>
       <c r="J24" s="113">
         <v>1</v>
       </c>
       <c r="K24" s="129" t="s">
-        <v>261</v>
+        <v>18</v>
       </c>
       <c r="L24" s="113" t="s">
         <v>90</v>
@@ -5185,27 +5179,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="24" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="83" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="B25" s="129" t="s">
         <v>274</v>
       </c>
       <c r="C25" s="113" t="s">
-        <v>443</v>
-      </c>
-      <c r="D25" s="113"/>
+        <v>456</v>
+      </c>
+      <c r="D25" s="114"/>
       <c r="E25" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F25" s="129" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="113" t="s">
+      <c r="H25" s="129" t="s">
         <v>344</v>
       </c>
       <c r="I25" s="129" t="s">
@@ -5215,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="129" t="s">
-        <v>261</v>
+        <v>422</v>
       </c>
       <c r="L25" s="113" t="s">
         <v>90</v>
@@ -5234,19 +5228,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:23" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="83" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="B26" s="129" t="s">
         <v>275</v>
       </c>
       <c r="C26" s="113" t="s">
-        <v>444</v>
-      </c>
-      <c r="D26" s="113"/>
+        <v>457</v>
+      </c>
+      <c r="D26" s="114"/>
       <c r="E26" s="114" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="F26" s="129" t="s">
         <v>291</v>
@@ -5254,11 +5248,11 @@
       <c r="G26" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="113" t="s">
-        <v>344</v>
+      <c r="H26" s="129" t="s">
+        <v>287</v>
       </c>
       <c r="I26" s="129" t="s">
-        <v>402</v>
+        <v>263</v>
       </c>
       <c r="J26" s="113">
         <v>1</v>
@@ -5283,37 +5277,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:23" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="83" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="B27" s="129" t="s">
         <v>276</v>
       </c>
       <c r="C27" s="113" t="s">
-        <v>445</v>
-      </c>
-      <c r="D27" s="113"/>
+        <v>458</v>
+      </c>
+      <c r="D27" s="114"/>
       <c r="E27" s="114" t="s">
-        <v>417</v>
-      </c>
-      <c r="F27" s="129" t="s">
-        <v>291</v>
+        <v>430</v>
+      </c>
+      <c r="F27" s="115" t="s">
+        <v>262</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="113" t="s">
+      <c r="H27" s="129" t="s">
         <v>344</v>
       </c>
       <c r="I27" s="129" t="s">
-        <v>402</v>
+        <v>243</v>
       </c>
       <c r="J27" s="113">
         <v>1</v>
       </c>
       <c r="K27" s="129" t="s">
-        <v>261</v>
+        <v>182</v>
       </c>
       <c r="L27" s="113" t="s">
         <v>90</v>
@@ -5332,37 +5326,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:23" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="83" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="B28" s="129" t="s">
         <v>277</v>
       </c>
       <c r="C28" s="113" t="s">
-        <v>446</v>
-      </c>
-      <c r="D28" s="113"/>
+        <v>459</v>
+      </c>
+      <c r="D28" s="114"/>
       <c r="E28" s="114" t="s">
-        <v>417</v>
-      </c>
-      <c r="F28" s="129" t="s">
-        <v>291</v>
+        <v>430</v>
+      </c>
+      <c r="F28" s="115" t="s">
+        <v>262</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="113" t="s">
-        <v>344</v>
+      <c r="H28" s="129" t="s">
+        <v>287</v>
       </c>
       <c r="I28" s="129" t="s">
-        <v>402</v>
+        <v>244</v>
       </c>
       <c r="J28" s="113">
         <v>1</v>
       </c>
       <c r="K28" s="129" t="s">
-        <v>261</v>
+        <v>18</v>
       </c>
       <c r="L28" s="113" t="s">
         <v>90</v>
@@ -5385,7 +5379,7 @@
       <c r="A29" s="83"/>
       <c r="B29" s="130"/>
       <c r="C29" s="113"/>
-      <c r="D29" s="113"/>
+      <c r="D29" s="114"/>
       <c r="E29" s="114"/>
       <c r="F29" s="115"/>
       <c r="G29" s="18"/>
@@ -5412,7 +5406,7 @@
       <c r="A30" s="83"/>
       <c r="B30" s="113"/>
       <c r="C30" s="113"/>
-      <c r="D30" s="113"/>
+      <c r="D30" s="114"/>
       <c r="E30" s="114"/>
       <c r="F30" s="115"/>
       <c r="G30" s="18"/>
@@ -5439,7 +5433,7 @@
       <c r="A31" s="83"/>
       <c r="B31" s="113"/>
       <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
+      <c r="D31" s="114"/>
       <c r="E31" s="114"/>
       <c r="F31" s="115"/>
       <c r="G31" s="18"/>
@@ -5466,7 +5460,7 @@
       <c r="A32" s="83"/>
       <c r="B32" s="113"/>
       <c r="C32" s="113"/>
-      <c r="D32" s="113"/>
+      <c r="D32" s="114"/>
       <c r="E32" s="114"/>
       <c r="F32" s="115"/>
       <c r="G32" s="18"/>
@@ -5493,7 +5487,7 @@
       <c r="A33" s="83"/>
       <c r="B33" s="113"/>
       <c r="C33" s="113"/>
-      <c r="D33" s="113"/>
+      <c r="D33" s="114"/>
       <c r="E33" s="114"/>
       <c r="F33" s="115"/>
       <c r="G33" s="18"/>
@@ -5520,7 +5514,7 @@
       <c r="A34" s="83"/>
       <c r="B34" s="113"/>
       <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
+      <c r="D34" s="114"/>
       <c r="E34" s="114"/>
       <c r="F34" s="115"/>
       <c r="G34" s="18"/>
@@ -5547,7 +5541,7 @@
       <c r="A35" s="83"/>
       <c r="B35" s="113"/>
       <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
+      <c r="D35" s="114"/>
       <c r="E35" s="114"/>
       <c r="F35" s="115"/>
       <c r="G35" s="18"/>
@@ -5574,7 +5568,7 @@
       <c r="A36" s="83"/>
       <c r="B36" s="113"/>
       <c r="C36" s="113"/>
-      <c r="D36" s="113"/>
+      <c r="D36" s="114"/>
       <c r="E36" s="114"/>
       <c r="F36" s="115"/>
       <c r="G36" s="18"/>
@@ -5601,7 +5595,7 @@
       <c r="A37" s="83"/>
       <c r="B37" s="113"/>
       <c r="C37" s="113"/>
-      <c r="D37" s="113"/>
+      <c r="D37" s="114"/>
       <c r="E37" s="114"/>
       <c r="F37" s="115"/>
       <c r="G37" s="18"/>
@@ -5628,7 +5622,7 @@
       <c r="A38" s="83"/>
       <c r="B38" s="113"/>
       <c r="C38" s="113"/>
-      <c r="D38" s="113"/>
+      <c r="D38" s="114"/>
       <c r="E38" s="114"/>
       <c r="F38" s="115"/>
       <c r="G38" s="18"/>
@@ -5655,7 +5649,7 @@
       <c r="A39" s="83"/>
       <c r="B39" s="113"/>
       <c r="C39" s="113"/>
-      <c r="D39" s="113"/>
+      <c r="D39" s="114"/>
       <c r="E39" s="114"/>
       <c r="F39" s="115"/>
       <c r="G39" s="18"/>
@@ -5682,7 +5676,7 @@
       <c r="A40" s="83"/>
       <c r="B40" s="113"/>
       <c r="C40" s="113"/>
-      <c r="D40" s="113"/>
+      <c r="D40" s="114"/>
       <c r="E40" s="114"/>
       <c r="F40" s="115"/>
       <c r="G40" s="18"/>
@@ -5709,7 +5703,7 @@
       <c r="A41" s="83"/>
       <c r="B41" s="113"/>
       <c r="C41" s="113"/>
-      <c r="D41" s="113"/>
+      <c r="D41" s="114"/>
       <c r="E41" s="114"/>
       <c r="F41" s="115"/>
       <c r="G41" s="18"/>
@@ -5736,7 +5730,7 @@
       <c r="A42" s="83"/>
       <c r="B42" s="113"/>
       <c r="C42" s="113"/>
-      <c r="D42" s="113"/>
+      <c r="D42" s="114"/>
       <c r="E42" s="114"/>
       <c r="F42" s="115"/>
       <c r="G42" s="18"/>
@@ -5763,7 +5757,7 @@
       <c r="A43" s="83"/>
       <c r="B43" s="113"/>
       <c r="C43" s="113"/>
-      <c r="D43" s="113"/>
+      <c r="D43" s="114"/>
       <c r="E43" s="114"/>
       <c r="F43" s="115"/>
       <c r="G43" s="18"/>
@@ -5790,7 +5784,7 @@
       <c r="A44" s="83"/>
       <c r="B44" s="113"/>
       <c r="C44" s="113"/>
-      <c r="D44" s="113"/>
+      <c r="D44" s="114"/>
       <c r="E44" s="114"/>
       <c r="F44" s="115"/>
       <c r="G44" s="18"/>
@@ -5817,7 +5811,7 @@
       <c r="A45" s="83"/>
       <c r="B45" s="113"/>
       <c r="C45" s="113"/>
-      <c r="D45" s="113"/>
+      <c r="D45" s="114"/>
       <c r="E45" s="114"/>
       <c r="F45" s="115"/>
       <c r="G45" s="18"/>
@@ -5844,7 +5838,7 @@
       <c r="A46" s="83"/>
       <c r="B46" s="113"/>
       <c r="C46" s="113"/>
-      <c r="D46" s="113"/>
+      <c r="D46" s="114"/>
       <c r="E46" s="114"/>
       <c r="F46" s="115"/>
       <c r="G46" s="18"/>
@@ -5871,7 +5865,7 @@
       <c r="A47" s="83"/>
       <c r="B47" s="113"/>
       <c r="C47" s="113"/>
-      <c r="D47" s="113"/>
+      <c r="D47" s="114"/>
       <c r="E47" s="114"/>
       <c r="F47" s="115"/>
       <c r="G47" s="18"/>
@@ -5898,7 +5892,7 @@
       <c r="A48" s="83"/>
       <c r="B48" s="113"/>
       <c r="C48" s="113"/>
-      <c r="D48" s="113"/>
+      <c r="D48" s="114"/>
       <c r="E48" s="114"/>
       <c r="F48" s="115"/>
       <c r="G48" s="18"/>
@@ -5925,7 +5919,7 @@
       <c r="A49" s="83"/>
       <c r="B49" s="113"/>
       <c r="C49" s="113"/>
-      <c r="D49" s="113"/>
+      <c r="D49" s="114"/>
       <c r="E49" s="114"/>
       <c r="F49" s="115"/>
       <c r="G49" s="18"/>
@@ -5952,7 +5946,7 @@
       <c r="A50" s="83"/>
       <c r="B50" s="113"/>
       <c r="C50" s="113"/>
-      <c r="D50" s="113"/>
+      <c r="D50" s="114"/>
       <c r="E50" s="114"/>
       <c r="F50" s="115"/>
       <c r="G50" s="18"/>
@@ -5979,7 +5973,7 @@
       <c r="A51" s="83"/>
       <c r="B51" s="113"/>
       <c r="C51" s="113"/>
-      <c r="D51" s="113"/>
+      <c r="D51" s="114"/>
       <c r="E51" s="114"/>
       <c r="F51" s="115"/>
       <c r="G51" s="18"/>
@@ -6006,7 +6000,7 @@
       <c r="A52" s="83"/>
       <c r="B52" s="113"/>
       <c r="C52" s="113"/>
-      <c r="D52" s="113"/>
+      <c r="D52" s="114"/>
       <c r="E52" s="114"/>
       <c r="F52" s="115"/>
       <c r="G52" s="18"/>
@@ -6033,7 +6027,7 @@
       <c r="A53" s="83"/>
       <c r="B53" s="113"/>
       <c r="C53" s="113"/>
-      <c r="D53" s="113"/>
+      <c r="D53" s="114"/>
       <c r="E53" s="114"/>
       <c r="F53" s="115"/>
       <c r="G53" s="18"/>
@@ -6060,7 +6054,7 @@
       <c r="A54" s="83"/>
       <c r="B54" s="113"/>
       <c r="C54" s="113"/>
-      <c r="D54" s="113"/>
+      <c r="D54" s="114"/>
       <c r="E54" s="114"/>
       <c r="F54" s="115"/>
       <c r="G54" s="18"/>
@@ -6087,7 +6081,7 @@
       <c r="A55" s="83"/>
       <c r="B55" s="113"/>
       <c r="C55" s="113"/>
-      <c r="D55" s="113"/>
+      <c r="D55" s="114"/>
       <c r="E55" s="114"/>
       <c r="F55" s="115"/>
       <c r="G55" s="18"/>
@@ -6114,7 +6108,7 @@
       <c r="A56" s="83"/>
       <c r="B56" s="113"/>
       <c r="C56" s="113"/>
-      <c r="D56" s="113"/>
+      <c r="D56" s="114"/>
       <c r="E56" s="114"/>
       <c r="F56" s="115"/>
       <c r="G56" s="18"/>
@@ -6141,7 +6135,7 @@
       <c r="A57" s="83"/>
       <c r="B57" s="113"/>
       <c r="C57" s="113"/>
-      <c r="D57" s="113"/>
+      <c r="D57" s="114"/>
       <c r="E57" s="114"/>
       <c r="F57" s="115"/>
       <c r="G57" s="18"/>
@@ -6168,7 +6162,7 @@
       <c r="A58" s="83"/>
       <c r="B58" s="113"/>
       <c r="C58" s="113"/>
-      <c r="D58" s="113"/>
+      <c r="D58" s="114"/>
       <c r="E58" s="114"/>
       <c r="F58" s="115"/>
       <c r="G58" s="18"/>
@@ -6195,7 +6189,7 @@
       <c r="A59" s="83"/>
       <c r="B59" s="113"/>
       <c r="C59" s="113"/>
-      <c r="D59" s="113"/>
+      <c r="D59" s="114"/>
       <c r="E59" s="114"/>
       <c r="F59" s="115"/>
       <c r="G59" s="18"/>
@@ -6222,7 +6216,7 @@
       <c r="A60" s="83"/>
       <c r="B60" s="113"/>
       <c r="C60" s="113"/>
-      <c r="D60" s="113"/>
+      <c r="D60" s="114"/>
       <c r="E60" s="114"/>
       <c r="F60" s="115"/>
       <c r="G60" s="18"/>
@@ -6249,7 +6243,7 @@
       <c r="A61" s="83"/>
       <c r="B61" s="113"/>
       <c r="C61" s="113"/>
-      <c r="D61" s="113"/>
+      <c r="D61" s="114"/>
       <c r="E61" s="114"/>
       <c r="F61" s="115"/>
       <c r="G61" s="18"/>
@@ -6276,7 +6270,7 @@
       <c r="A62" s="83"/>
       <c r="B62" s="113"/>
       <c r="C62" s="113"/>
-      <c r="D62" s="113"/>
+      <c r="D62" s="114"/>
       <c r="E62" s="114"/>
       <c r="F62" s="115"/>
       <c r="G62" s="18"/>
@@ -6303,7 +6297,7 @@
       <c r="A63" s="83"/>
       <c r="B63" s="113"/>
       <c r="C63" s="113"/>
-      <c r="D63" s="113"/>
+      <c r="D63" s="114"/>
       <c r="E63" s="114"/>
       <c r="F63" s="115"/>
       <c r="G63" s="18"/>
@@ -6330,7 +6324,7 @@
       <c r="A64" s="83"/>
       <c r="B64" s="113"/>
       <c r="C64" s="113"/>
-      <c r="D64" s="113"/>
+      <c r="D64" s="114"/>
       <c r="E64" s="114"/>
       <c r="F64" s="115"/>
       <c r="G64" s="18"/>
@@ -6357,7 +6351,7 @@
       <c r="A65" s="83"/>
       <c r="B65" s="113"/>
       <c r="C65" s="113"/>
-      <c r="D65" s="113"/>
+      <c r="D65" s="114"/>
       <c r="E65" s="114"/>
       <c r="F65" s="115"/>
       <c r="G65" s="18"/>
@@ -6384,7 +6378,7 @@
       <c r="A66" s="83"/>
       <c r="B66" s="113"/>
       <c r="C66" s="113"/>
-      <c r="D66" s="113"/>
+      <c r="D66" s="114"/>
       <c r="E66" s="114"/>
       <c r="F66" s="115"/>
       <c r="G66" s="18"/>
@@ -6411,7 +6405,7 @@
       <c r="A67" s="83"/>
       <c r="B67" s="113"/>
       <c r="C67" s="113"/>
-      <c r="D67" s="113"/>
+      <c r="D67" s="114"/>
       <c r="E67" s="114"/>
       <c r="F67" s="115"/>
       <c r="G67" s="18"/>
@@ -6438,7 +6432,7 @@
       <c r="A68" s="83"/>
       <c r="B68" s="113"/>
       <c r="C68" s="113"/>
-      <c r="D68" s="113"/>
+      <c r="D68" s="114"/>
       <c r="E68" s="114"/>
       <c r="F68" s="115"/>
       <c r="G68" s="18"/>
@@ -6465,7 +6459,7 @@
       <c r="A69" s="83"/>
       <c r="B69" s="113"/>
       <c r="C69" s="113"/>
-      <c r="D69" s="113"/>
+      <c r="D69" s="114"/>
       <c r="E69" s="114"/>
       <c r="F69" s="115"/>
       <c r="G69" s="18"/>
@@ -6492,7 +6486,7 @@
       <c r="A70" s="83"/>
       <c r="B70" s="113"/>
       <c r="C70" s="113"/>
-      <c r="D70" s="113"/>
+      <c r="D70" s="114"/>
       <c r="E70" s="114"/>
       <c r="F70" s="115"/>
       <c r="G70" s="18"/>
@@ -6519,7 +6513,7 @@
       <c r="A71" s="83"/>
       <c r="B71" s="113"/>
       <c r="C71" s="113"/>
-      <c r="D71" s="113"/>
+      <c r="D71" s="114"/>
       <c r="E71" s="114"/>
       <c r="F71" s="115"/>
       <c r="G71" s="18"/>
@@ -6546,7 +6540,7 @@
       <c r="A72" s="83"/>
       <c r="B72" s="113"/>
       <c r="C72" s="113"/>
-      <c r="D72" s="113"/>
+      <c r="D72" s="114"/>
       <c r="E72" s="114"/>
       <c r="F72" s="115"/>
       <c r="G72" s="18"/>
@@ -6573,7 +6567,7 @@
       <c r="A73" s="83"/>
       <c r="B73" s="113"/>
       <c r="C73" s="113"/>
-      <c r="D73" s="113"/>
+      <c r="D73" s="114"/>
       <c r="E73" s="114"/>
       <c r="F73" s="115"/>
       <c r="G73" s="18"/>
@@ -6600,7 +6594,7 @@
       <c r="A74" s="83"/>
       <c r="B74" s="113"/>
       <c r="C74" s="113"/>
-      <c r="D74" s="113"/>
+      <c r="D74" s="114"/>
       <c r="E74" s="114"/>
       <c r="F74" s="115"/>
       <c r="G74" s="18"/>
@@ -6627,7 +6621,7 @@
       <c r="A75" s="83"/>
       <c r="B75" s="113"/>
       <c r="C75" s="113"/>
-      <c r="D75" s="113"/>
+      <c r="D75" s="114"/>
       <c r="E75" s="114"/>
       <c r="F75" s="115"/>
       <c r="G75" s="18"/>
@@ -6654,7 +6648,7 @@
       <c r="A76" s="83"/>
       <c r="B76" s="113"/>
       <c r="C76" s="113"/>
-      <c r="D76" s="113"/>
+      <c r="D76" s="114"/>
       <c r="E76" s="114"/>
       <c r="F76" s="115"/>
       <c r="G76" s="18"/>
@@ -6681,7 +6675,7 @@
       <c r="A77" s="83"/>
       <c r="B77" s="113"/>
       <c r="C77" s="113"/>
-      <c r="D77" s="113"/>
+      <c r="D77" s="114"/>
       <c r="E77" s="114"/>
       <c r="F77" s="115"/>
       <c r="G77" s="18"/>
@@ -6708,7 +6702,7 @@
       <c r="A78" s="83"/>
       <c r="B78" s="113"/>
       <c r="C78" s="113"/>
-      <c r="D78" s="113"/>
+      <c r="D78" s="114"/>
       <c r="E78" s="114"/>
       <c r="F78" s="115"/>
       <c r="G78" s="18"/>
@@ -6735,7 +6729,7 @@
       <c r="A79" s="83"/>
       <c r="B79" s="113"/>
       <c r="C79" s="113"/>
-      <c r="D79" s="113"/>
+      <c r="D79" s="114"/>
       <c r="E79" s="114"/>
       <c r="F79" s="115"/>
       <c r="G79" s="18"/>
@@ -6762,7 +6756,7 @@
       <c r="A80" s="83"/>
       <c r="B80" s="113"/>
       <c r="C80" s="113"/>
-      <c r="D80" s="113"/>
+      <c r="D80" s="114"/>
       <c r="E80" s="114"/>
       <c r="F80" s="115"/>
       <c r="G80" s="18"/>
@@ -6789,7 +6783,7 @@
       <c r="A81" s="83"/>
       <c r="B81" s="113"/>
       <c r="C81" s="113"/>
-      <c r="D81" s="113"/>
+      <c r="D81" s="114"/>
       <c r="E81" s="114"/>
       <c r="F81" s="115"/>
       <c r="G81" s="18"/>
@@ -6816,7 +6810,7 @@
       <c r="A82" s="83"/>
       <c r="B82" s="113"/>
       <c r="C82" s="113"/>
-      <c r="D82" s="113"/>
+      <c r="D82" s="114"/>
       <c r="E82" s="114"/>
       <c r="F82" s="115"/>
       <c r="G82" s="18"/>
@@ -6843,7 +6837,7 @@
       <c r="A83" s="83"/>
       <c r="B83" s="113"/>
       <c r="C83" s="113"/>
-      <c r="D83" s="113"/>
+      <c r="D83" s="114"/>
       <c r="E83" s="114"/>
       <c r="F83" s="115"/>
       <c r="G83" s="18"/>
@@ -6870,7 +6864,7 @@
       <c r="A84" s="83"/>
       <c r="B84" s="113"/>
       <c r="C84" s="113"/>
-      <c r="D84" s="113"/>
+      <c r="D84" s="114"/>
       <c r="E84" s="114"/>
       <c r="F84" s="115"/>
       <c r="G84" s="18"/>
@@ -6897,7 +6891,7 @@
       <c r="A85" s="83"/>
       <c r="B85" s="113"/>
       <c r="C85" s="113"/>
-      <c r="D85" s="113"/>
+      <c r="D85" s="114"/>
       <c r="E85" s="114"/>
       <c r="F85" s="115"/>
       <c r="G85" s="18"/>
@@ -6924,7 +6918,7 @@
       <c r="A86" s="83"/>
       <c r="B86" s="113"/>
       <c r="C86" s="113"/>
-      <c r="D86" s="113"/>
+      <c r="D86" s="114"/>
       <c r="E86" s="114"/>
       <c r="F86" s="115"/>
       <c r="G86" s="18"/>
@@ -6951,7 +6945,7 @@
       <c r="A87" s="83"/>
       <c r="B87" s="113"/>
       <c r="C87" s="113"/>
-      <c r="D87" s="113"/>
+      <c r="D87" s="114"/>
       <c r="E87" s="114"/>
       <c r="F87" s="115"/>
       <c r="G87" s="18"/>
@@ -6978,7 +6972,7 @@
       <c r="A88" s="83"/>
       <c r="B88" s="113"/>
       <c r="C88" s="113"/>
-      <c r="D88" s="113"/>
+      <c r="D88" s="114"/>
       <c r="E88" s="114"/>
       <c r="F88" s="115"/>
       <c r="G88" s="18"/>
@@ -7005,7 +6999,7 @@
       <c r="A89" s="83"/>
       <c r="B89" s="113"/>
       <c r="C89" s="113"/>
-      <c r="D89" s="113"/>
+      <c r="D89" s="114"/>
       <c r="E89" s="114"/>
       <c r="F89" s="115"/>
       <c r="G89" s="18"/>
@@ -7032,7 +7026,7 @@
       <c r="A90" s="83"/>
       <c r="B90" s="113"/>
       <c r="C90" s="113"/>
-      <c r="D90" s="113"/>
+      <c r="D90" s="114"/>
       <c r="E90" s="114"/>
       <c r="F90" s="115"/>
       <c r="G90" s="18"/>
@@ -7059,7 +7053,7 @@
       <c r="A91" s="83"/>
       <c r="B91" s="113"/>
       <c r="C91" s="113"/>
-      <c r="D91" s="113"/>
+      <c r="D91" s="114"/>
       <c r="E91" s="114"/>
       <c r="F91" s="115"/>
       <c r="G91" s="18"/>
@@ -7086,7 +7080,7 @@
       <c r="A92" s="83"/>
       <c r="B92" s="113"/>
       <c r="C92" s="113"/>
-      <c r="D92" s="113"/>
+      <c r="D92" s="114"/>
       <c r="E92" s="114"/>
       <c r="F92" s="115"/>
       <c r="G92" s="18"/>
@@ -7113,7 +7107,7 @@
       <c r="A93" s="83"/>
       <c r="B93" s="113"/>
       <c r="C93" s="113"/>
-      <c r="D93" s="113"/>
+      <c r="D93" s="114"/>
       <c r="E93" s="114"/>
       <c r="F93" s="115"/>
       <c r="G93" s="18"/>
@@ -7140,7 +7134,7 @@
       <c r="A94" s="83"/>
       <c r="B94" s="113"/>
       <c r="C94" s="113"/>
-      <c r="D94" s="113"/>
+      <c r="D94" s="114"/>
       <c r="E94" s="114"/>
       <c r="F94" s="115"/>
       <c r="G94" s="18"/>
@@ -7167,7 +7161,7 @@
       <c r="A95" s="83"/>
       <c r="B95" s="113"/>
       <c r="C95" s="113"/>
-      <c r="D95" s="113"/>
+      <c r="D95" s="114"/>
       <c r="E95" s="114"/>
       <c r="F95" s="115"/>
       <c r="G95" s="18"/>
@@ -7194,7 +7188,7 @@
       <c r="A96" s="83"/>
       <c r="B96" s="113"/>
       <c r="C96" s="113"/>
-      <c r="D96" s="113"/>
+      <c r="D96" s="114"/>
       <c r="E96" s="114"/>
       <c r="F96" s="115"/>
       <c r="G96" s="18"/>
@@ -7221,7 +7215,7 @@
       <c r="A97" s="83"/>
       <c r="B97" s="113"/>
       <c r="C97" s="113"/>
-      <c r="D97" s="113"/>
+      <c r="D97" s="114"/>
       <c r="E97" s="114"/>
       <c r="F97" s="115"/>
       <c r="G97" s="18"/>
@@ -7248,7 +7242,7 @@
       <c r="A98" s="83"/>
       <c r="B98" s="113"/>
       <c r="C98" s="113"/>
-      <c r="D98" s="113"/>
+      <c r="D98" s="114"/>
       <c r="E98" s="114"/>
       <c r="F98" s="115"/>
       <c r="G98" s="18"/>
@@ -7275,7 +7269,7 @@
       <c r="A99" s="83"/>
       <c r="B99" s="113"/>
       <c r="C99" s="113"/>
-      <c r="D99" s="113"/>
+      <c r="D99" s="114"/>
       <c r="E99" s="114"/>
       <c r="F99" s="115"/>
       <c r="G99" s="18"/>
@@ -7302,7 +7296,7 @@
       <c r="A100" s="83"/>
       <c r="B100" s="113"/>
       <c r="C100" s="113"/>
-      <c r="D100" s="113"/>
+      <c r="D100" s="114"/>
       <c r="E100" s="114"/>
       <c r="F100" s="115"/>
       <c r="G100" s="18"/>
@@ -7329,7 +7323,7 @@
       <c r="A101" s="83"/>
       <c r="B101" s="113"/>
       <c r="C101" s="113"/>
-      <c r="D101" s="113"/>
+      <c r="D101" s="114"/>
       <c r="E101" s="114"/>
       <c r="F101" s="115"/>
       <c r="G101" s="18"/>
@@ -7356,7 +7350,7 @@
       <c r="A102" s="83"/>
       <c r="B102" s="113"/>
       <c r="C102" s="113"/>
-      <c r="D102" s="113"/>
+      <c r="D102" s="114"/>
       <c r="E102" s="114"/>
       <c r="F102" s="115"/>
       <c r="G102" s="18"/>
@@ -7383,7 +7377,7 @@
       <c r="A103" s="83"/>
       <c r="B103" s="113"/>
       <c r="C103" s="113"/>
-      <c r="D103" s="113"/>
+      <c r="D103" s="114"/>
       <c r="E103" s="114"/>
       <c r="F103" s="115"/>
       <c r="G103" s="18"/>
@@ -7410,7 +7404,7 @@
       <c r="A104" s="83"/>
       <c r="B104" s="113"/>
       <c r="C104" s="113"/>
-      <c r="D104" s="113"/>
+      <c r="D104" s="114"/>
       <c r="E104" s="114"/>
       <c r="F104" s="115"/>
       <c r="G104" s="18"/>
@@ -7437,7 +7431,7 @@
       <c r="A105" s="83"/>
       <c r="B105" s="113"/>
       <c r="C105" s="113"/>
-      <c r="D105" s="113"/>
+      <c r="D105" s="114"/>
       <c r="E105" s="114"/>
       <c r="F105" s="115"/>
       <c r="G105" s="18"/>
@@ -7464,7 +7458,7 @@
       <c r="A106" s="83"/>
       <c r="B106" s="113"/>
       <c r="C106" s="113"/>
-      <c r="D106" s="113"/>
+      <c r="D106" s="114"/>
       <c r="E106" s="114"/>
       <c r="F106" s="115"/>
       <c r="G106" s="18"/>
@@ -7491,7 +7485,7 @@
       <c r="A107" s="83"/>
       <c r="B107" s="113"/>
       <c r="C107" s="113"/>
-      <c r="D107" s="113"/>
+      <c r="D107" s="114"/>
       <c r="E107" s="114"/>
       <c r="F107" s="115"/>
       <c r="G107" s="18"/>
@@ -7518,7 +7512,7 @@
       <c r="A108" s="83"/>
       <c r="B108" s="113"/>
       <c r="C108" s="113"/>
-      <c r="D108" s="113"/>
+      <c r="D108" s="114"/>
       <c r="E108" s="114"/>
       <c r="F108" s="115"/>
       <c r="G108" s="18"/>
@@ -7545,7 +7539,7 @@
       <c r="A109" s="83"/>
       <c r="B109" s="113"/>
       <c r="C109" s="113"/>
-      <c r="D109" s="113"/>
+      <c r="D109" s="114"/>
       <c r="E109" s="114"/>
       <c r="F109" s="115"/>
       <c r="G109" s="18"/>
@@ -7572,7 +7566,7 @@
       <c r="A110" s="83"/>
       <c r="B110" s="113"/>
       <c r="C110" s="113"/>
-      <c r="D110" s="113"/>
+      <c r="D110" s="114"/>
       <c r="E110" s="114"/>
       <c r="F110" s="115"/>
       <c r="G110" s="18"/>
@@ -7599,7 +7593,7 @@
       <c r="A111" s="83"/>
       <c r="B111" s="113"/>
       <c r="C111" s="113"/>
-      <c r="D111" s="113"/>
+      <c r="D111" s="114"/>
       <c r="E111" s="114"/>
       <c r="F111" s="115"/>
       <c r="G111" s="18"/>
@@ -7626,7 +7620,7 @@
       <c r="A112" s="83"/>
       <c r="B112" s="113"/>
       <c r="C112" s="113"/>
-      <c r="D112" s="113"/>
+      <c r="D112" s="114"/>
       <c r="E112" s="114"/>
       <c r="F112" s="115"/>
       <c r="G112" s="18"/>
@@ -7653,7 +7647,7 @@
       <c r="A113" s="83"/>
       <c r="B113" s="113"/>
       <c r="C113" s="113"/>
-      <c r="D113" s="113"/>
+      <c r="D113" s="114"/>
       <c r="E113" s="114"/>
       <c r="F113" s="115"/>
       <c r="G113" s="18"/>
@@ -7680,7 +7674,7 @@
       <c r="A114" s="83"/>
       <c r="B114" s="113"/>
       <c r="C114" s="113"/>
-      <c r="D114" s="113"/>
+      <c r="D114" s="114"/>
       <c r="E114" s="114"/>
       <c r="F114" s="115"/>
       <c r="G114" s="18"/>
@@ -7707,7 +7701,7 @@
       <c r="A115" s="83"/>
       <c r="B115" s="113"/>
       <c r="C115" s="113"/>
-      <c r="D115" s="113"/>
+      <c r="D115" s="114"/>
       <c r="E115" s="114"/>
       <c r="F115" s="115"/>
       <c r="G115" s="18"/>
@@ -7734,7 +7728,7 @@
       <c r="A116" s="83"/>
       <c r="B116" s="113"/>
       <c r="C116" s="113"/>
-      <c r="D116" s="113"/>
+      <c r="D116" s="114"/>
       <c r="E116" s="114"/>
       <c r="F116" s="115"/>
       <c r="G116" s="18"/>
@@ -7761,7 +7755,7 @@
       <c r="A117" s="83"/>
       <c r="B117" s="113"/>
       <c r="C117" s="113"/>
-      <c r="D117" s="113"/>
+      <c r="D117" s="114"/>
       <c r="E117" s="114"/>
       <c r="F117" s="115"/>
       <c r="G117" s="18"/>
@@ -7788,7 +7782,7 @@
       <c r="A118" s="83"/>
       <c r="B118" s="113"/>
       <c r="C118" s="113"/>
-      <c r="D118" s="113"/>
+      <c r="D118" s="114"/>
       <c r="E118" s="114"/>
       <c r="F118" s="115"/>
       <c r="G118" s="18"/>
@@ -7815,7 +7809,7 @@
       <c r="A119" s="83"/>
       <c r="B119" s="113"/>
       <c r="C119" s="113"/>
-      <c r="D119" s="113"/>
+      <c r="D119" s="114"/>
       <c r="E119" s="114"/>
       <c r="F119" s="115"/>
       <c r="G119" s="18"/>
@@ -7842,7 +7836,7 @@
       <c r="A120" s="83"/>
       <c r="B120" s="113"/>
       <c r="C120" s="113"/>
-      <c r="D120" s="113"/>
+      <c r="D120" s="114"/>
       <c r="E120" s="114"/>
       <c r="F120" s="115"/>
       <c r="G120" s="18"/>
@@ -7867,7 +7861,7 @@
       <c r="A121" s="83"/>
       <c r="B121" s="113"/>
       <c r="C121" s="113"/>
-      <c r="D121" s="113"/>
+      <c r="D121" s="114"/>
       <c r="E121" s="114"/>
       <c r="F121" s="115"/>
       <c r="G121" s="18"/>
@@ -7892,7 +7886,7 @@
       <c r="A122" s="83"/>
       <c r="B122" s="113"/>
       <c r="C122" s="113"/>
-      <c r="D122" s="113"/>
+      <c r="D122" s="114"/>
       <c r="E122" s="114"/>
       <c r="F122" s="115"/>
       <c r="G122" s="18"/>
@@ -7917,7 +7911,7 @@
       <c r="A123" s="83"/>
       <c r="B123" s="113"/>
       <c r="C123" s="113"/>
-      <c r="D123" s="113"/>
+      <c r="D123" s="114"/>
       <c r="E123" s="114"/>
       <c r="F123" s="115"/>
       <c r="G123" s="18"/>
@@ -7942,7 +7936,7 @@
       <c r="A124" s="83"/>
       <c r="B124" s="113"/>
       <c r="C124" s="113"/>
-      <c r="D124" s="113"/>
+      <c r="D124" s="114"/>
       <c r="E124" s="114"/>
       <c r="F124" s="115"/>
       <c r="G124" s="18"/>
@@ -7967,7 +7961,7 @@
       <c r="A125" s="83"/>
       <c r="B125" s="113"/>
       <c r="C125" s="113"/>
-      <c r="D125" s="113"/>
+      <c r="D125" s="114"/>
       <c r="E125" s="114"/>
       <c r="F125" s="115"/>
       <c r="G125" s="18"/>
@@ -7992,7 +7986,7 @@
       <c r="A126" s="83"/>
       <c r="B126" s="113"/>
       <c r="C126" s="113"/>
-      <c r="D126" s="113"/>
+      <c r="D126" s="114"/>
       <c r="E126" s="114"/>
       <c r="F126" s="115"/>
       <c r="G126" s="18"/>
@@ -8017,7 +8011,7 @@
       <c r="A127" s="83"/>
       <c r="B127" s="113"/>
       <c r="C127" s="113"/>
-      <c r="D127" s="113"/>
+      <c r="D127" s="114"/>
       <c r="E127" s="114"/>
       <c r="F127" s="115"/>
       <c r="G127" s="18"/>
@@ -8042,7 +8036,7 @@
       <c r="A128" s="83"/>
       <c r="B128" s="113"/>
       <c r="C128" s="113"/>
-      <c r="D128" s="113"/>
+      <c r="D128" s="114"/>
       <c r="E128" s="114"/>
       <c r="F128" s="115"/>
       <c r="G128" s="18"/>
@@ -8067,7 +8061,7 @@
       <c r="A129" s="83"/>
       <c r="B129" s="113"/>
       <c r="C129" s="113"/>
-      <c r="D129" s="113"/>
+      <c r="D129" s="114"/>
       <c r="E129" s="114"/>
       <c r="F129" s="115"/>
       <c r="G129" s="18"/>
@@ -8092,7 +8086,7 @@
       <c r="A130" s="83"/>
       <c r="B130" s="113"/>
       <c r="C130" s="113"/>
-      <c r="D130" s="113"/>
+      <c r="D130" s="114"/>
       <c r="E130" s="114"/>
       <c r="F130" s="115"/>
       <c r="G130" s="18"/>
@@ -8117,7 +8111,7 @@
       <c r="A131" s="83"/>
       <c r="B131" s="113"/>
       <c r="C131" s="113"/>
-      <c r="D131" s="113"/>
+      <c r="D131" s="114"/>
       <c r="E131" s="114"/>
       <c r="F131" s="115"/>
       <c r="G131" s="18"/>
@@ -8142,7 +8136,7 @@
       <c r="A132" s="83"/>
       <c r="B132" s="113"/>
       <c r="C132" s="113"/>
-      <c r="D132" s="113"/>
+      <c r="D132" s="114"/>
       <c r="E132" s="114"/>
       <c r="F132" s="115"/>
       <c r="G132" s="18"/>
@@ -8167,7 +8161,7 @@
       <c r="A133" s="83"/>
       <c r="B133" s="113"/>
       <c r="C133" s="113"/>
-      <c r="D133" s="113"/>
+      <c r="D133" s="114"/>
       <c r="E133" s="114"/>
       <c r="F133" s="115"/>
       <c r="G133" s="18"/>
@@ -8192,7 +8186,7 @@
       <c r="A134" s="83"/>
       <c r="B134" s="113"/>
       <c r="C134" s="113"/>
-      <c r="D134" s="113"/>
+      <c r="D134" s="114"/>
       <c r="E134" s="114"/>
       <c r="F134" s="115"/>
       <c r="G134" s="18"/>
@@ -8217,7 +8211,7 @@
       <c r="A135" s="83"/>
       <c r="B135" s="113"/>
       <c r="C135" s="113"/>
-      <c r="D135" s="113"/>
+      <c r="D135" s="114"/>
       <c r="E135" s="114"/>
       <c r="F135" s="115"/>
       <c r="G135" s="18"/>
@@ -8242,7 +8236,7 @@
       <c r="A136" s="83"/>
       <c r="B136" s="113"/>
       <c r="C136" s="113"/>
-      <c r="D136" s="113"/>
+      <c r="D136" s="114"/>
       <c r="E136" s="114"/>
       <c r="F136" s="115"/>
       <c r="G136" s="18"/>
@@ -8267,7 +8261,7 @@
       <c r="A137" s="83"/>
       <c r="B137" s="113"/>
       <c r="C137" s="113"/>
-      <c r="D137" s="113"/>
+      <c r="D137" s="114"/>
       <c r="E137" s="114"/>
       <c r="F137" s="115"/>
       <c r="G137" s="18"/>
@@ -8292,7 +8286,7 @@
       <c r="A138" s="83"/>
       <c r="B138" s="113"/>
       <c r="C138" s="113"/>
-      <c r="D138" s="113"/>
+      <c r="D138" s="114"/>
       <c r="E138" s="114"/>
       <c r="F138" s="115"/>
       <c r="G138" s="18"/>
@@ -8317,7 +8311,7 @@
       <c r="A139" s="83"/>
       <c r="B139" s="113"/>
       <c r="C139" s="113"/>
-      <c r="D139" s="113"/>
+      <c r="D139" s="114"/>
       <c r="E139" s="114"/>
       <c r="F139" s="115"/>
       <c r="G139" s="18"/>
@@ -8342,7 +8336,7 @@
       <c r="A140" s="83"/>
       <c r="B140" s="113"/>
       <c r="C140" s="113"/>
-      <c r="D140" s="113"/>
+      <c r="D140" s="114"/>
       <c r="E140" s="114"/>
       <c r="F140" s="115"/>
       <c r="G140" s="18"/>
@@ -8367,7 +8361,7 @@
       <c r="A141" s="83"/>
       <c r="B141" s="113"/>
       <c r="C141" s="113"/>
-      <c r="D141" s="113"/>
+      <c r="D141" s="114"/>
       <c r="E141" s="114"/>
       <c r="F141" s="115"/>
       <c r="G141" s="18"/>
@@ -8392,7 +8386,7 @@
       <c r="A142" s="83"/>
       <c r="B142" s="113"/>
       <c r="C142" s="113"/>
-      <c r="D142" s="113"/>
+      <c r="D142" s="114"/>
       <c r="E142" s="114"/>
       <c r="F142" s="115"/>
       <c r="G142" s="18"/>
@@ -8417,7 +8411,7 @@
       <c r="A143" s="83"/>
       <c r="B143" s="113"/>
       <c r="C143" s="113"/>
-      <c r="D143" s="113"/>
+      <c r="D143" s="114"/>
       <c r="E143" s="114"/>
       <c r="F143" s="115"/>
       <c r="G143" s="18"/>
@@ -8442,7 +8436,7 @@
       <c r="A144" s="83"/>
       <c r="B144" s="113"/>
       <c r="C144" s="113"/>
-      <c r="D144" s="113"/>
+      <c r="D144" s="114"/>
       <c r="E144" s="114"/>
       <c r="F144" s="115"/>
       <c r="G144" s="18"/>
@@ -8467,7 +8461,7 @@
       <c r="A145" s="83"/>
       <c r="B145" s="113"/>
       <c r="C145" s="113"/>
-      <c r="D145" s="113"/>
+      <c r="D145" s="114"/>
       <c r="E145" s="114"/>
       <c r="F145" s="115"/>
       <c r="G145" s="18"/>
@@ -8492,7 +8486,7 @@
       <c r="A146" s="83"/>
       <c r="B146" s="113"/>
       <c r="C146" s="113"/>
-      <c r="D146" s="113"/>
+      <c r="D146" s="114"/>
       <c r="E146" s="114"/>
       <c r="F146" s="115"/>
       <c r="G146" s="18"/>
@@ -8517,7 +8511,7 @@
       <c r="A147" s="83"/>
       <c r="B147" s="113"/>
       <c r="C147" s="113"/>
-      <c r="D147" s="113"/>
+      <c r="D147" s="114"/>
       <c r="E147" s="114"/>
       <c r="F147" s="115"/>
       <c r="G147" s="18"/>
@@ -8542,7 +8536,7 @@
       <c r="A148" s="83"/>
       <c r="B148" s="113"/>
       <c r="C148" s="113"/>
-      <c r="D148" s="113"/>
+      <c r="D148" s="114"/>
       <c r="E148" s="114"/>
       <c r="F148" s="115"/>
       <c r="G148" s="18"/>
@@ -8567,7 +8561,7 @@
       <c r="A149" s="83"/>
       <c r="B149" s="113"/>
       <c r="C149" s="113"/>
-      <c r="D149" s="113"/>
+      <c r="D149" s="114"/>
       <c r="E149" s="114"/>
       <c r="F149" s="115"/>
       <c r="G149" s="18"/>
@@ -8592,7 +8586,7 @@
       <c r="A150" s="83"/>
       <c r="B150" s="113"/>
       <c r="C150" s="113"/>
-      <c r="D150" s="113"/>
+      <c r="D150" s="114"/>
       <c r="E150" s="114"/>
       <c r="F150" s="115"/>
       <c r="G150" s="18"/>
@@ -8617,7 +8611,7 @@
       <c r="A151" s="83"/>
       <c r="B151" s="113"/>
       <c r="C151" s="113"/>
-      <c r="D151" s="113"/>
+      <c r="D151" s="114"/>
       <c r="E151" s="114"/>
       <c r="F151" s="115"/>
       <c r="G151" s="18"/>
@@ -8642,7 +8636,7 @@
       <c r="A152" s="83"/>
       <c r="B152" s="113"/>
       <c r="C152" s="113"/>
-      <c r="D152" s="113"/>
+      <c r="D152" s="114"/>
       <c r="E152" s="114"/>
       <c r="F152" s="115"/>
       <c r="G152" s="18"/>
@@ -8667,7 +8661,7 @@
       <c r="A153" s="83"/>
       <c r="B153" s="113"/>
       <c r="C153" s="113"/>
-      <c r="D153" s="113"/>
+      <c r="D153" s="114"/>
       <c r="E153" s="114"/>
       <c r="F153" s="115"/>
       <c r="G153" s="18"/>
@@ -8692,7 +8686,7 @@
       <c r="A154" s="83"/>
       <c r="B154" s="113"/>
       <c r="C154" s="113"/>
-      <c r="D154" s="113"/>
+      <c r="D154" s="114"/>
       <c r="E154" s="114"/>
       <c r="F154" s="115"/>
       <c r="G154" s="18"/>
@@ -8717,7 +8711,7 @@
       <c r="A155" s="83"/>
       <c r="B155" s="113"/>
       <c r="C155" s="113"/>
-      <c r="D155" s="113"/>
+      <c r="D155" s="114"/>
       <c r="E155" s="114"/>
       <c r="F155" s="115"/>
       <c r="G155" s="18"/>
@@ -8742,7 +8736,7 @@
       <c r="A156" s="83"/>
       <c r="B156" s="113"/>
       <c r="C156" s="113"/>
-      <c r="D156" s="113"/>
+      <c r="D156" s="114"/>
       <c r="E156" s="114"/>
       <c r="F156" s="115"/>
       <c r="G156" s="18"/>
@@ -8767,7 +8761,7 @@
       <c r="A157" s="83"/>
       <c r="B157" s="113"/>
       <c r="C157" s="113"/>
-      <c r="D157" s="113"/>
+      <c r="D157" s="114"/>
       <c r="E157" s="114"/>
       <c r="F157" s="115"/>
       <c r="G157" s="18"/>
@@ -8792,7 +8786,7 @@
       <c r="A158" s="83"/>
       <c r="B158" s="113"/>
       <c r="C158" s="113"/>
-      <c r="D158" s="113"/>
+      <c r="D158" s="114"/>
       <c r="E158" s="114"/>
       <c r="F158" s="115"/>
       <c r="G158" s="18"/>
@@ -8817,7 +8811,7 @@
       <c r="A159" s="83"/>
       <c r="B159" s="113"/>
       <c r="C159" s="113"/>
-      <c r="D159" s="113"/>
+      <c r="D159" s="114"/>
       <c r="E159" s="114"/>
       <c r="F159" s="115"/>
       <c r="G159" s="18"/>
@@ -8842,7 +8836,7 @@
       <c r="A160" s="83"/>
       <c r="B160" s="113"/>
       <c r="C160" s="113"/>
-      <c r="D160" s="113"/>
+      <c r="D160" s="114"/>
       <c r="E160" s="114"/>
       <c r="F160" s="115"/>
       <c r="G160" s="18"/>
@@ -8867,7 +8861,7 @@
       <c r="A161" s="83"/>
       <c r="B161" s="113"/>
       <c r="C161" s="113"/>
-      <c r="D161" s="113"/>
+      <c r="D161" s="114"/>
       <c r="E161" s="114"/>
       <c r="F161" s="115"/>
       <c r="G161" s="18"/>
@@ -8892,7 +8886,7 @@
       <c r="A162" s="83"/>
       <c r="B162" s="113"/>
       <c r="C162" s="113"/>
-      <c r="D162" s="113"/>
+      <c r="D162" s="114"/>
       <c r="E162" s="114"/>
       <c r="F162" s="115"/>
       <c r="G162" s="18"/>
@@ -8917,7 +8911,7 @@
       <c r="A163" s="83"/>
       <c r="B163" s="113"/>
       <c r="C163" s="113"/>
-      <c r="D163" s="113"/>
+      <c r="D163" s="114"/>
       <c r="E163" s="114"/>
       <c r="F163" s="115"/>
       <c r="G163" s="18"/>
@@ -8942,7 +8936,7 @@
       <c r="A164" s="83"/>
       <c r="B164" s="113"/>
       <c r="C164" s="113"/>
-      <c r="D164" s="113"/>
+      <c r="D164" s="114"/>
       <c r="E164" s="114"/>
       <c r="F164" s="115"/>
       <c r="G164" s="18"/>
@@ -8967,7 +8961,7 @@
       <c r="A165" s="83"/>
       <c r="B165" s="113"/>
       <c r="C165" s="113"/>
-      <c r="D165" s="113"/>
+      <c r="D165" s="114"/>
       <c r="E165" s="114"/>
       <c r="F165" s="115"/>
       <c r="G165" s="18"/>
@@ -8992,7 +8986,7 @@
       <c r="A166" s="83"/>
       <c r="B166" s="113"/>
       <c r="C166" s="113"/>
-      <c r="D166" s="113"/>
+      <c r="D166" s="114"/>
       <c r="E166" s="114"/>
       <c r="F166" s="115"/>
       <c r="G166" s="18"/>
@@ -9017,7 +9011,7 @@
       <c r="A167" s="83"/>
       <c r="B167" s="113"/>
       <c r="C167" s="113"/>
-      <c r="D167" s="113"/>
+      <c r="D167" s="114"/>
       <c r="E167" s="114"/>
       <c r="F167" s="115"/>
       <c r="G167" s="18"/>
@@ -9042,7 +9036,7 @@
       <c r="A168" s="83"/>
       <c r="B168" s="113"/>
       <c r="C168" s="113"/>
-      <c r="D168" s="113"/>
+      <c r="D168" s="114"/>
       <c r="E168" s="114"/>
       <c r="F168" s="115"/>
       <c r="G168" s="18"/>
@@ -9067,7 +9061,7 @@
       <c r="A169" s="83"/>
       <c r="B169" s="113"/>
       <c r="C169" s="113"/>
-      <c r="D169" s="113"/>
+      <c r="D169" s="114"/>
       <c r="E169" s="114"/>
       <c r="F169" s="115"/>
       <c r="G169" s="18"/>
@@ -9092,7 +9086,7 @@
       <c r="A170" s="83"/>
       <c r="B170" s="113"/>
       <c r="C170" s="113"/>
-      <c r="D170" s="113"/>
+      <c r="D170" s="114"/>
       <c r="E170" s="114"/>
       <c r="F170" s="115"/>
       <c r="G170" s="18"/>
@@ -9117,7 +9111,7 @@
       <c r="A171" s="83"/>
       <c r="B171" s="113"/>
       <c r="C171" s="113"/>
-      <c r="D171" s="113"/>
+      <c r="D171" s="114"/>
       <c r="E171" s="114"/>
       <c r="F171" s="115"/>
       <c r="G171" s="18"/>
@@ -9142,7 +9136,7 @@
       <c r="A172" s="83"/>
       <c r="B172" s="113"/>
       <c r="C172" s="113"/>
-      <c r="D172" s="113"/>
+      <c r="D172" s="114"/>
       <c r="E172" s="114"/>
       <c r="F172" s="115"/>
       <c r="G172" s="18"/>
@@ -9167,7 +9161,7 @@
       <c r="A173" s="83"/>
       <c r="B173" s="113"/>
       <c r="C173" s="113"/>
-      <c r="D173" s="113"/>
+      <c r="D173" s="114"/>
       <c r="E173" s="114"/>
       <c r="F173" s="115"/>
       <c r="G173" s="18"/>
@@ -9192,7 +9186,7 @@
       <c r="A174" s="83"/>
       <c r="B174" s="113"/>
       <c r="C174" s="113"/>
-      <c r="D174" s="113"/>
+      <c r="D174" s="114"/>
       <c r="E174" s="114"/>
       <c r="F174" s="115"/>
       <c r="G174" s="18"/>
@@ -9217,7 +9211,7 @@
       <c r="A175" s="83"/>
       <c r="B175" s="113"/>
       <c r="C175" s="113"/>
-      <c r="D175" s="113"/>
+      <c r="D175" s="114"/>
       <c r="E175" s="114"/>
       <c r="F175" s="115"/>
       <c r="G175" s="18"/>
@@ -9242,7 +9236,7 @@
       <c r="A176" s="83"/>
       <c r="B176" s="113"/>
       <c r="C176" s="113"/>
-      <c r="D176" s="113"/>
+      <c r="D176" s="114"/>
       <c r="E176" s="114"/>
       <c r="F176" s="115"/>
       <c r="G176" s="18"/>
@@ -9267,7 +9261,7 @@
       <c r="A177" s="83"/>
       <c r="B177" s="113"/>
       <c r="C177" s="113"/>
-      <c r="D177" s="113"/>
+      <c r="D177" s="114"/>
       <c r="E177" s="114"/>
       <c r="F177" s="115"/>
       <c r="G177" s="18"/>
@@ -9292,7 +9286,7 @@
       <c r="A178" s="83"/>
       <c r="B178" s="113"/>
       <c r="C178" s="113"/>
-      <c r="D178" s="113"/>
+      <c r="D178" s="114"/>
       <c r="E178" s="114"/>
       <c r="F178" s="115"/>
       <c r="G178" s="18"/>
@@ -9317,7 +9311,7 @@
       <c r="A179" s="83"/>
       <c r="B179" s="113"/>
       <c r="C179" s="113"/>
-      <c r="D179" s="113"/>
+      <c r="D179" s="114"/>
       <c r="E179" s="114"/>
       <c r="F179" s="115"/>
       <c r="G179" s="18"/>
@@ -9342,7 +9336,7 @@
       <c r="A180" s="83"/>
       <c r="B180" s="113"/>
       <c r="C180" s="113"/>
-      <c r="D180" s="113"/>
+      <c r="D180" s="114"/>
       <c r="E180" s="114"/>
       <c r="F180" s="115"/>
       <c r="G180" s="18"/>
@@ -9367,7 +9361,7 @@
       <c r="A181" s="83"/>
       <c r="B181" s="113"/>
       <c r="C181" s="113"/>
-      <c r="D181" s="113"/>
+      <c r="D181" s="114"/>
       <c r="E181" s="114"/>
       <c r="F181" s="115"/>
       <c r="G181" s="18"/>
@@ -9392,7 +9386,7 @@
       <c r="A182" s="83"/>
       <c r="B182" s="113"/>
       <c r="C182" s="113"/>
-      <c r="D182" s="113"/>
+      <c r="D182" s="114"/>
       <c r="E182" s="114"/>
       <c r="F182" s="115"/>
       <c r="G182" s="18"/>
@@ -9417,7 +9411,7 @@
       <c r="A183" s="83"/>
       <c r="B183" s="113"/>
       <c r="C183" s="113"/>
-      <c r="D183" s="113"/>
+      <c r="D183" s="114"/>
       <c r="E183" s="114"/>
       <c r="F183" s="115"/>
       <c r="G183" s="18"/>
@@ -9442,7 +9436,7 @@
       <c r="A184" s="83"/>
       <c r="B184" s="113"/>
       <c r="C184" s="113"/>
-      <c r="D184" s="113"/>
+      <c r="D184" s="114"/>
       <c r="E184" s="114"/>
       <c r="F184" s="115"/>
       <c r="G184" s="18"/>
@@ -9467,7 +9461,7 @@
       <c r="A185" s="83"/>
       <c r="B185" s="113"/>
       <c r="C185" s="113"/>
-      <c r="D185" s="113"/>
+      <c r="D185" s="114"/>
       <c r="E185" s="114"/>
       <c r="F185" s="115"/>
       <c r="G185" s="18"/>
@@ -9494,7 +9488,7 @@
       <c r="A186" s="83"/>
       <c r="B186" s="113"/>
       <c r="C186" s="113"/>
-      <c r="D186" s="113"/>
+      <c r="D186" s="114"/>
       <c r="E186" s="114"/>
       <c r="F186" s="115"/>
       <c r="G186" s="18"/>
@@ -9521,7 +9515,7 @@
       <c r="A187" s="83"/>
       <c r="B187" s="113"/>
       <c r="C187" s="113"/>
-      <c r="D187" s="113"/>
+      <c r="D187" s="114"/>
       <c r="E187" s="114"/>
       <c r="F187" s="115"/>
       <c r="G187" s="18"/>
@@ -9548,7 +9542,7 @@
       <c r="A188" s="83"/>
       <c r="B188" s="113"/>
       <c r="C188" s="113"/>
-      <c r="D188" s="113"/>
+      <c r="D188" s="114"/>
       <c r="E188" s="114"/>
       <c r="F188" s="115"/>
       <c r="G188" s="18"/>
@@ -9575,7 +9569,7 @@
       <c r="A189" s="83"/>
       <c r="B189" s="113"/>
       <c r="C189" s="113"/>
-      <c r="D189" s="113"/>
+      <c r="D189" s="114"/>
       <c r="E189" s="114"/>
       <c r="F189" s="115"/>
       <c r="G189" s="18"/>
@@ -9602,7 +9596,7 @@
       <c r="A190" s="83"/>
       <c r="B190" s="113"/>
       <c r="C190" s="113"/>
-      <c r="D190" s="113"/>
+      <c r="D190" s="114"/>
       <c r="E190" s="114"/>
       <c r="F190" s="115"/>
       <c r="G190" s="18"/>
@@ -9629,7 +9623,7 @@
       <c r="A191" s="83"/>
       <c r="B191" s="113"/>
       <c r="C191" s="113"/>
-      <c r="D191" s="113"/>
+      <c r="D191" s="114"/>
       <c r="E191" s="114"/>
       <c r="F191" s="115"/>
       <c r="G191" s="18"/>
@@ -9656,7 +9650,7 @@
       <c r="A192" s="83"/>
       <c r="B192" s="113"/>
       <c r="C192" s="113"/>
-      <c r="D192" s="113"/>
+      <c r="D192" s="114"/>
       <c r="E192" s="114"/>
       <c r="F192" s="115"/>
       <c r="G192" s="18"/>
@@ -9683,7 +9677,7 @@
       <c r="A193" s="83"/>
       <c r="B193" s="113"/>
       <c r="C193" s="113"/>
-      <c r="D193" s="113"/>
+      <c r="D193" s="114"/>
       <c r="E193" s="114"/>
       <c r="F193" s="115"/>
       <c r="G193" s="18"/>
@@ -9710,7 +9704,7 @@
       <c r="A194" s="83"/>
       <c r="B194" s="113"/>
       <c r="C194" s="113"/>
-      <c r="D194" s="113"/>
+      <c r="D194" s="114"/>
       <c r="E194" s="114"/>
       <c r="F194" s="115"/>
       <c r="G194" s="18"/>
@@ -9737,7 +9731,7 @@
       <c r="A195" s="83"/>
       <c r="B195" s="113"/>
       <c r="C195" s="113"/>
-      <c r="D195" s="113"/>
+      <c r="D195" s="114"/>
       <c r="E195" s="114"/>
       <c r="F195" s="115"/>
       <c r="G195" s="18"/>
@@ -9764,7 +9758,7 @@
       <c r="A196" s="83"/>
       <c r="B196" s="113"/>
       <c r="C196" s="113"/>
-      <c r="D196" s="113"/>
+      <c r="D196" s="114"/>
       <c r="E196" s="114"/>
       <c r="F196" s="115"/>
       <c r="G196" s="18"/>
@@ -9791,7 +9785,7 @@
       <c r="A197" s="83"/>
       <c r="B197" s="113"/>
       <c r="C197" s="113"/>
-      <c r="D197" s="113"/>
+      <c r="D197" s="114"/>
       <c r="E197" s="114"/>
       <c r="F197" s="115"/>
       <c r="G197" s="18"/>
@@ -9818,7 +9812,7 @@
       <c r="A198" s="83"/>
       <c r="B198" s="113"/>
       <c r="C198" s="113"/>
-      <c r="D198" s="113"/>
+      <c r="D198" s="114"/>
       <c r="E198" s="114"/>
       <c r="F198" s="115"/>
       <c r="G198" s="18"/>
@@ -9845,7 +9839,7 @@
       <c r="A199" s="83"/>
       <c r="B199" s="113"/>
       <c r="C199" s="113"/>
-      <c r="D199" s="113"/>
+      <c r="D199" s="114"/>
       <c r="E199" s="114"/>
       <c r="F199" s="115"/>
       <c r="G199" s="18"/>
@@ -9872,7 +9866,7 @@
       <c r="A200" s="83"/>
       <c r="B200" s="113"/>
       <c r="C200" s="113"/>
-      <c r="D200" s="113"/>
+      <c r="D200" s="114"/>
       <c r="E200" s="114"/>
       <c r="F200" s="115"/>
       <c r="G200" s="18"/>
@@ -9901,7 +9895,7 @@
       </c>
       <c r="B201" s="117"/>
       <c r="C201" s="117"/>
-      <c r="D201" s="117"/>
+      <c r="D201" s="114"/>
       <c r="F201" s="115"/>
       <c r="J201" s="113"/>
       <c r="R201" s="72"/>
@@ -10000,20 +9994,19 @@
       <c r="R232" s="72"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="jVwmeeyZ3/5JcZTNYDZQQIUFBpYP4Fl8es9UmfABo2cB6dPI/ayUpVNmomsf2XPtxnEZWebG+sDDAPEjEb5NZQ==" saltValue="Kp69cNwM/UXB4htjtM0LTQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="S9:U9"/>
     <mergeCell ref="N9:O9"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations xWindow="64075" yWindow="65218" count="4">
+  <dataValidations xWindow="64075" yWindow="65218" count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use accession number from NCBI (e.g NC_000001)" sqref="C15:C200" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W14:W200" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Only required if &quot;Other&quot; is chosen in column &quot;Species&quot;." sqref="Q15:R200" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Use accession number from NCBI (e.g NC_000001)" sqref="D18:D200 D15:D16" xr:uid="{87E50626-C876-BC4C-84A7-A443368AC7E8}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -10026,7 +10019,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="64075" yWindow="65218" count="10">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="64075" yWindow="65218" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!#REF!</xm:f>
@@ -10038,12 +10031,6 @@
             <xm:f>'Drop down list'!$J$2:$J$97</xm:f>
           </x14:formula1>
           <xm:sqref>O15:P200</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If sample is in buffer with EDTA, contact Clinical genomics before submission." xr:uid="{4D767856-33F8-EA44-B848-D2D194C17FA1}">
-          <x14:formula1>
-            <xm:f>'Drop down list'!$F$2:$F$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H15:H200</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
@@ -10081,11 +10068,23 @@
           </x14:formula1>
           <xm:sqref>F15:F201</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{958EA2DC-9655-B244-968A-7D24319BCCA9}">
+          <x14:formula1>
+            <xm:f>'Drop down list'!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D15:D201</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If &quot;Other&quot;, specify in &quot;Other species&quot; field." xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>'Drop down list'!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>B30:B200 B15:B28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If sample is in buffer with EDTA, contact Clinical genomics before submission." xr:uid="{4D767856-33F8-EA44-B848-D2D194C17FA1}">
+          <x14:formula1>
+            <xm:f>'Drop down list'!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H19:H200 H15:H17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10101,7 +10100,7 @@
   <dimension ref="A1:N203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10122,7 +10121,7 @@
         <v>260</v>
       </c>
       <c r="B1" s="121" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" s="118" t="s">
         <v>409</v>
@@ -10153,9 +10152,6 @@
       <c r="A2" s="71" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="71" t="s">
-        <v>421</v>
-      </c>
       <c r="C2" s="71" t="s">
         <v>412</v>
       </c>
@@ -10186,10 +10182,10 @@
         <v>268</v>
       </c>
       <c r="B3" s="71" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="D3" s="71" t="s">
         <v>289</v>
@@ -10218,7 +10214,7 @@
         <v>269</v>
       </c>
       <c r="B4" s="71" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D4" s="71" t="s">
         <v>290</v>
@@ -10233,7 +10229,7 @@
         <v>244</v>
       </c>
       <c r="H4" s="71" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J4" s="71" t="s">
         <v>27</v>
@@ -11588,7 +11584,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="nyg8Gl7ZiHg5J4oACW44Q+6mSzjz6iiqfPhLjAucG4cCHYQ+v0a9FrIlSnEGPD8A1McmTXNUXvSV2e9tqIRYMA==" saltValue="dbry7tw+9R8JTS+3UVS3cg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="e20PgIxDi6ynXmjnSCPcn+qOehgxufAIu0OKWvRnCyztsEl827OhTT4s1JrLcALkhEhq1cEPk7tIV1FSz198Cw==" saltValue="rFk+/NRGe6NV/G3y0piozg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>